<commit_message>
Made it more CHAP compatible and wrote more README
</commit_message>
<xml_diff>
--- a/input/env_info.xlsx
+++ b/input/env_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Halvard\Documents\GitHub\epidemiar\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F4A1A66F-8F3B-4A93-BD61-53C4F75C6A02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB09ED9A-E8C8-4F00-A524-C3CC2A7C626C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2250" yWindow="2250" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="environ_info" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
   <si>
     <t>environ_var_code</t>
   </si>
@@ -83,6 +83,12 @@
   </si>
   <si>
     <t>lst_night</t>
+  </si>
+  <si>
+    <t>mean_temperature</t>
+  </si>
+  <si>
+    <t>rainfall</t>
   </si>
 </sst>
 </file>
@@ -889,15 +895,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
   </cols>
@@ -915,7 +921,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -926,7 +932,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -937,18 +943,18 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -959,56 +965,78 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
       </c>
       <c r="C10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Made the model compatible with weekly data
The model now runs with weekly data from CHAP. Might still be worse than if given daily data
</commit_message>
<xml_diff>
--- a/input/env_info.xlsx
+++ b/input/env_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Halvard\Documents\GitHub\epidemiar\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB09ED9A-E8C8-4F00-A524-C3CC2A7C626C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE884770-D754-41DA-BA13-F72EA717880D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2685" yWindow="2685" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="environ_info" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
   <si>
     <t>environ_var_code</t>
   </si>
@@ -29,9 +29,6 @@
   </si>
   <si>
     <t>report_label</t>
-  </si>
-  <si>
-    <t>sum</t>
   </si>
   <si>
     <t>Rain (mm)</t>
@@ -897,8 +894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -921,123 +918,123 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
         <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
         <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
         <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
         <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
         <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
         <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
         <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
         <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
         <v>13</v>
-      </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
         <v>15</v>
-      </c>
-      <c r="B12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>